<commit_message>
Starbucks Map Crawling & Visualizing
</commit_message>
<xml_diff>
--- a/Selenium/Starbucks/df_seoul_final.xlsx
+++ b/Selenium/Starbucks/df_seoul_final.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>시군구코드</t>
   </si>
@@ -26,6 +26,306 @@
   </si>
   <si>
     <t>경도</t>
+  </si>
+  <si>
+    <t>11320</t>
+  </si>
+  <si>
+    <t>11380</t>
+  </si>
+  <si>
+    <t>11230</t>
+  </si>
+  <si>
+    <t>11590</t>
+  </si>
+  <si>
+    <t>11545</t>
+  </si>
+  <si>
+    <t>11530</t>
+  </si>
+  <si>
+    <t>11110</t>
+  </si>
+  <si>
+    <t>11305</t>
+  </si>
+  <si>
+    <t>11260</t>
+  </si>
+  <si>
+    <t>11680</t>
+  </si>
+  <si>
+    <t>11500</t>
+  </si>
+  <si>
+    <t>11140</t>
+  </si>
+  <si>
+    <t>11740</t>
+  </si>
+  <si>
+    <t>11215</t>
+  </si>
+  <si>
+    <t>11440</t>
+  </si>
+  <si>
+    <t>11650</t>
+  </si>
+  <si>
+    <t>11290</t>
+  </si>
+  <si>
+    <t>11350</t>
+  </si>
+  <si>
+    <t>11710</t>
+  </si>
+  <si>
+    <t>11410</t>
+  </si>
+  <si>
+    <t>11470</t>
+  </si>
+  <si>
+    <t>11560</t>
+  </si>
+  <si>
+    <t>11620</t>
+  </si>
+  <si>
+    <t>11200</t>
+  </si>
+  <si>
+    <t>11170</t>
+  </si>
+  <si>
+    <t>도봉구</t>
+  </si>
+  <si>
+    <t>은평구</t>
+  </si>
+  <si>
+    <t>동대문구</t>
+  </si>
+  <si>
+    <t>동작구</t>
+  </si>
+  <si>
+    <t>금천구</t>
+  </si>
+  <si>
+    <t>구로구</t>
+  </si>
+  <si>
+    <t>종로구</t>
+  </si>
+  <si>
+    <t>강북구</t>
+  </si>
+  <si>
+    <t>중랑구</t>
+  </si>
+  <si>
+    <t>강남구</t>
+  </si>
+  <si>
+    <t>강서구</t>
+  </si>
+  <si>
+    <t>중구</t>
+  </si>
+  <si>
+    <t>강동구</t>
+  </si>
+  <si>
+    <t>광진구</t>
+  </si>
+  <si>
+    <t>마포구</t>
+  </si>
+  <si>
+    <t>서초구</t>
+  </si>
+  <si>
+    <t>성북구</t>
+  </si>
+  <si>
+    <t>노원구</t>
+  </si>
+  <si>
+    <t>송파구</t>
+  </si>
+  <si>
+    <t>서대문구</t>
+  </si>
+  <si>
+    <t>양천구</t>
+  </si>
+  <si>
+    <t>영등포구</t>
+  </si>
+  <si>
+    <t>관악구</t>
+  </si>
+  <si>
+    <t>성동구</t>
+  </si>
+  <si>
+    <t>용산구</t>
+  </si>
+  <si>
+    <t>37.6658609</t>
+  </si>
+  <si>
+    <t>37.6176125</t>
+  </si>
+  <si>
+    <t>37.5838012</t>
+  </si>
+  <si>
+    <t>37.4965037</t>
+  </si>
+  <si>
+    <t>37.4600969</t>
+  </si>
+  <si>
+    <t>37.4954856</t>
+  </si>
+  <si>
+    <t>37.5990998</t>
+  </si>
+  <si>
+    <t>37.6469954</t>
+  </si>
+  <si>
+    <t>37.5953795</t>
+  </si>
+  <si>
+    <t>37.4959854</t>
+  </si>
+  <si>
+    <t>37.5657617</t>
+  </si>
+  <si>
+    <t>37.5579452</t>
+  </si>
+  <si>
+    <t>37.5492077</t>
+  </si>
+  <si>
+    <t>37.5481445</t>
+  </si>
+  <si>
+    <t>37.5622906</t>
+  </si>
+  <si>
+    <t>37.4769528</t>
+  </si>
+  <si>
+    <t>37.606991</t>
+  </si>
+  <si>
+    <t>37.655264</t>
+  </si>
+  <si>
+    <t>37.5048534</t>
+  </si>
+  <si>
+    <t>37.5820369</t>
+  </si>
+  <si>
+    <t>37.5270616</t>
+  </si>
+  <si>
+    <t>37.520641</t>
+  </si>
+  <si>
+    <t>37.4653993</t>
+  </si>
+  <si>
+    <t>37.5506753</t>
+  </si>
+  <si>
+    <t>37.5311008</t>
+  </si>
+  <si>
+    <t>127.0317674</t>
+  </si>
+  <si>
+    <t>126.9227004</t>
+  </si>
+  <si>
+    <t>127.0507003</t>
+  </si>
+  <si>
+    <t>126.9443073</t>
+  </si>
+  <si>
+    <t>126.9001546</t>
+  </si>
+  <si>
+    <t>126.858121</t>
+  </si>
+  <si>
+    <t>126.9861493</t>
+  </si>
+  <si>
+    <t>127.0147158</t>
+  </si>
+  <si>
+    <t>127.0939669</t>
+  </si>
+  <si>
+    <t>127.0664091</t>
+  </si>
+  <si>
+    <t>126.8226561</t>
+  </si>
+  <si>
+    <t>126.9941904</t>
+  </si>
+  <si>
+    <t>127.1464824</t>
+  </si>
+  <si>
+    <t>127.0857528</t>
+  </si>
+  <si>
+    <t>126.9087803</t>
+  </si>
+  <si>
+    <t>127.0378103</t>
+  </si>
+  <si>
+    <t>127.0232185</t>
+  </si>
+  <si>
+    <t>127.0771201</t>
+  </si>
+  <si>
+    <t>127.1144822</t>
+  </si>
+  <si>
+    <t>126.9356665</t>
+  </si>
+  <si>
+    <t>126.8561534</t>
+  </si>
+  <si>
+    <t>126.9139242</t>
+  </si>
+  <si>
+    <t>126.9438071</t>
+  </si>
+  <si>
+    <t>127.0409622</t>
+  </si>
+  <si>
+    <t>126.9810742</t>
   </si>
 </sst>
 </file>
@@ -383,7 +683,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -403,6 +703,356 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>